<commit_message>
CAMBIOS NUEVOS NUEVA LAPTOP
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/timbrado_logistic_s.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/timbrado_logistic_s.xlsx
@@ -1326,10 +1326,10 @@
   <dimension ref="A1:AB77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D43" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D37" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>